<commit_message>
Attendance marking functionality added
</commit_message>
<xml_diff>
--- a/database/attendance.xlsx
+++ b/database/attendance.xlsx
@@ -1,85 +1,48 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ksr/Documents/Kousthubha's Docs/Development/face_recognition_based_attendance/database/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A422E72B-9F6D-3043-9068-9F7D3593FE7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16080" xr2:uid="{4E2997DA-9A9F-E044-83A5-CE0D466BE713}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16080" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>StudentName</t>
-  </si>
-  <si>
-    <t>RollNo</t>
-  </si>
-  <si>
-    <t>Activity</t>
-  </si>
-  <si>
-    <t>STD1234</t>
-  </si>
-  <si>
-    <t>Kousthubha</t>
-  </si>
-  <si>
-    <t>LOGIN</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="166" formatCode="yyyy-mm-dd h:mm:ss"/>
+  </numFmts>
+  <fonts count="2">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="12"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -87,27 +50,106 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -407,44 +449,122 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18E5FACE-120C-3C49-8327-0D3EAFE3FD68}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col width="34.33203125" customWidth="1" min="1" max="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>RollNo</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>StudentName</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Activity</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>44696.691666666666</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
+    <row r="2">
+      <c r="A2" s="2" t="n">
+        <v>44696.79898611111</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>STD1234</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Kousthubha</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>LOGIN</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="n">
+        <v>44696.80397918981</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>STD1234</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Kousthubha</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>LOGOUT</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="n">
+        <v>44696.80630842593</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>STD1234</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Kousthubha</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>LOGIN</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="n">
+        <v>44696.80655411498</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>STD1234</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Kousthubha</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>LOGOUT</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>